<commit_message>
hotfix: remove label partition in top labeled venue
</commit_message>
<xml_diff>
--- a/jobs/etl_jobs/external/ppg/templates/export_template.xlsx
+++ b/jobs/etl_jobs/external/ppg/templates/export_template.xlsx
@@ -816,7 +816,7 @@
     <t>Nombre d'établissements éligibles</t>
   </si>
   <si>
-    <t>kpi_name = pct_partenaire_culturel_actif</t>
+    <t>kpi_name = taux_d_utilisation_du_credit</t>
   </si>
   <si>
     <t>Taux de conso (%)</t>
@@ -828,7 +828,7 @@
     <t>Montant théorique alloué</t>
   </si>
   <si>
-    <t>kpi_name = total_partenaire_avec_offre_vitrine</t>
+    <t>kpi_name = montant_moyen_par_reservation</t>
   </si>
   <si>
     <t>Montant moyen par réservation</t>
@@ -840,7 +840,7 @@
     <t>Dont engagé auprès d'AC du territoire</t>
   </si>
   <si>
-    <t>kpi_name = taux_d_utilisation_du_credit</t>
+    <t>kpi_name = pct_partenaire_culturel_actif</t>
   </si>
   <si>
     <t>Taux de couverture AC (%)</t>
@@ -852,7 +852,7 @@
     <t>Nombre d'AC activés (déjà publié une offre collective)</t>
   </si>
   <si>
-    <t>kpi_name = montant_moyen_par_reservation</t>
+    <t>kpi_name = total_partenaire_avec_offre_vitrine</t>
   </si>
   <si>
     <t>Nombre d'AC avec offres vitrines</t>
@@ -47781,7 +47781,7 @@
       <c r="G12" s="127"/>
       <c r="H12" s="127"/>
       <c r="I12" s="127"/>
-      <c r="J12" s="127"/>
+      <c r="J12" s="121"/>
       <c r="K12" s="127"/>
       <c r="L12" s="127"/>
       <c r="M12" s="127"/>
@@ -47800,6 +47800,7 @@
       <c r="C13" s="122"/>
       <c r="D13" s="129"/>
       <c r="F13" s="23"/>
+      <c r="J13" s="121"/>
     </row>
     <row r="14">
       <c r="A14" s="121" t="s">
@@ -47819,7 +47820,7 @@
       <c r="G14" s="124"/>
       <c r="H14" s="124"/>
       <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
+      <c r="J14" s="121"/>
       <c r="K14" s="124"/>
       <c r="L14" s="124"/>
       <c r="M14" s="124"/>
@@ -47850,7 +47851,7 @@
       <c r="G15" s="130"/>
       <c r="H15" s="130"/>
       <c r="I15" s="130"/>
-      <c r="J15" s="130"/>
+      <c r="J15" s="121"/>
       <c r="K15" s="130"/>
       <c r="L15" s="130"/>
       <c r="M15" s="130"/>

</xml_diff>